<commit_message>
npc spawn inner값 삭제
</commit_message>
<xml_diff>
--- a/spawn.xlsx
+++ b/spawn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\endgame\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47909A3F-FD71-4461-8D53-DA6B0A6A96C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F24E0D-187A-42EE-BECF-445216008168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{52B2F6BD-FAB0-4697-8424-EA8D96EDCB24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,10 +127,6 @@
   </si>
   <si>
     <t>spawn_criminal_outer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spawn_npc_inner</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -594,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72770396-C383-4002-8A15-9510EB2CAA31}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -626,7 +622,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -719,36 +715,25 @@
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
+        <v>130</v>
+      </c>
+      <c r="E7" s="5">
         <v>120</v>
       </c>
-      <c r="E7" s="5">
-        <v>56</v>
-      </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>130</v>
-      </c>
-      <c r="E8" s="5">
-        <v>120</v>
-      </c>
-      <c r="F8" s="6"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3"/>
@@ -771,13 +756,6 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>